<commit_message>
add and more results
</commit_message>
<xml_diff>
--- a/results/yq_test/qft_cz/Rb2Re4/cz_2q_qft_10.qasm_rb2_archsize4_mini_dis.xlsx
+++ b/results/yq_test/qft_cz/Rb2Re4/cz_2q_qft_10.qasm_rb2_archsize4_mini_dis.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N138"/>
+  <dimension ref="A1:N139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.03241705894470215</v>
+        <v>0.0006709098815917969</v>
       </c>
     </row>
     <row r="6">
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.002394914627075195</v>
+        <v>0.000560760498046875</v>
       </c>
     </row>
     <row r="7">
@@ -497,13 +497,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.001702070236206055</v>
+        <v>0.002531051635742188</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>[(2, 0), (1, 3), (0, 3), (0, 2), (0, 0), (2, 1), (1, 2), (1, 0), (1, 1), (0, 1)]</t>
+          <t>[[2, 0], [1, 3], [0, 3], [0, 2], [0, 0], [2, 1], [1, 2], [1, 0], [1, 1], [0, 1]]</t>
         </is>
       </c>
     </row>
@@ -793,7 +793,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>[(2, 1), (1, 1), (1, 2), (0, 2), (0, 3), (1, 3), (0, 1), (2, 2), (1, 0), (2, 0)]</t>
+          <t>[[2, 1], [1, 1], [1, 2], [0, 2], [0, 3], [1, 3], [0, 1], [2, 2], [1, 0], [2, 0]]</t>
         </is>
       </c>
     </row>
@@ -1148,7 +1148,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>[(1, 1), (0, 2), (0, 1), (0, 0), (1, 2), (1, 0), (2, 0), (0, 3), (1, 3), (2, 1)]</t>
+          <t>[[1, 1], [0, 2], [0, 1], [0, 0], [1, 2], [1, 0], [2, 0], [0, 3], [1, 3], [2, 1]]</t>
         </is>
       </c>
     </row>
@@ -1406,110 +1406,120 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Movement times</t>
+          <t>move_fidelity</t>
         </is>
       </c>
       <c r="B134" t="n">
-        <v>16</v>
+        <v>0.9990298597111551</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>parallel times</t>
+          <t>Movement times</t>
         </is>
       </c>
       <c r="B135" t="n">
-        <v>105</v>
+        <v>16</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>partitions</t>
+          <t>parallel times</t>
         </is>
       </c>
       <c r="B136" t="n">
-        <v>3</v>
+        <v>105</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>total time:</t>
+          <t>partitions</t>
         </is>
       </c>
       <c r="B137" t="n">
-        <v>0.04448676109313965</v>
+        <v>3</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
+          <t>total time:</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>0.01520490646362305</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
           <t>T_cz</t>
         </is>
       </c>
-      <c r="B138" t="inlineStr">
+      <c r="B139" t="inlineStr">
         <is>
           <t>0.2</t>
         </is>
       </c>
-      <c r="C138" t="inlineStr">
+      <c r="C139" t="inlineStr">
         <is>
           <t>T_eff</t>
         </is>
       </c>
-      <c r="D138" t="inlineStr">
+      <c r="D139" t="inlineStr">
         <is>
           <t>1500000.0</t>
         </is>
       </c>
-      <c r="E138" t="inlineStr">
+      <c r="E139" t="inlineStr">
         <is>
           <t>T_trans</t>
         </is>
       </c>
-      <c r="F138" t="inlineStr">
+      <c r="F139" t="inlineStr">
         <is>
           <t>20</t>
         </is>
       </c>
-      <c r="G138" t="inlineStr">
+      <c r="G139" t="inlineStr">
         <is>
           <t>AOD_width</t>
         </is>
       </c>
-      <c r="H138" t="inlineStr">
+      <c r="H139" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="I138" t="inlineStr">
+      <c r="I139" t="inlineStr">
         <is>
           <t>AOD_height</t>
         </is>
       </c>
-      <c r="J138" t="inlineStr">
+      <c r="J139" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="K138" t="inlineStr">
+      <c r="K139" t="inlineStr">
         <is>
           <t>Move_speed</t>
         </is>
       </c>
-      <c r="L138" t="inlineStr">
+      <c r="L139" t="inlineStr">
         <is>
           <t>0.55</t>
         </is>
       </c>
-      <c r="M138" t="inlineStr">
+      <c r="M139" t="inlineStr">
         <is>
           <t>F_cz</t>
         </is>
       </c>
-      <c r="N138" t="inlineStr">
+      <c r="N139" t="inlineStr">
         <is>
           <t>0.995</t>
         </is>

</xml_diff>